<commit_message>
Agregado Busqueda Binaria con bug
</commit_message>
<xml_diff>
--- a/TP 2/Archivos/CSV/Resultados Euler.xlsx
+++ b/TP 2/Archivos/CSV/Resultados Euler.xlsx
@@ -636,7 +636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>

</xml_diff>